<commit_message>
Add a new file for storing user data
Create an empty Excel file to store user input data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: aa1355a6-4859-4c24-8204-39ae879ef4a6
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/71061587-a7b1-4597-9e8f-9df05ef5f8e3/aa1355a6-4859-4c24-8204-39ae879ef4a6/JZWKwlC
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,14 +456,29 @@
           <t>Test User</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="B2" t="n">
+        <v>25</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Test submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>This is a test from the form</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user data with the latest information
The user_data.xlsx file has been updated.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: aa1355a6-4859-4c24-8204-39ae879ef4a6
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/71061587-a7b1-4597-9e8f-9df05ef5f8e3/aa1355a6-4859-4c24-8204-39ae879ef4a6/JZWKwlC
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,14 +471,29 @@
           <t>John Doe</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="B3" t="n">
+        <v>30</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>This is a test from the form</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>hii</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user data file with latest submissions
The user_data.xlsx file has been updated to reflect the latest form submissions.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: aa1355a6-4859-4c24-8204-39ae879ef4a6
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/71061587-a7b1-4597-9e8f-9df05ef5f8e3/aa1355a6-4859-4c24-8204-39ae879ef4a6/JZWKwlC
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,14 +486,29 @@
           <t>hi</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="B4" t="n">
+        <v>5</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>hii</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TestGB</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>hi</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve data handling by ensuring Excel file compatibility
Update `app.py` to explicitly use the `openpyxl` engine for reading and writing Excel files, addressing potential compatibility issues and ensuring data integrity when the file is not initially present or when appending new records.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: aa1355a6-4859-4c24-8204-39ae879ef4a6
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/71061587-a7b1-4597-9e8f-9df05ef5f8e3/aa1355a6-4859-4c24-8204-39ae879ef4a6/9cIJIDv
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,62 +453,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Test User</t>
+          <t>Test User Fixed</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Test submission</t>
+          <t>First submission after fix</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>30</v>
+          <t>Second Test</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>This is a test from the form</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>hi</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>hii</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TestGB</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>hi</t>
+          <t>Testing multiple entries</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update success message to be more concise
Changes the success alert message from "Submitted successfully!" to "data is submitted" in index.html.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: aa1355a6-4859-4c24-8204-39ae879ef4a6
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/71061587-a7b1-4597-9e8f-9df05ef5f8e3/aa1355a6-4859-4c24-8204-39ae879ef4a6/9cIJIDv
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,14 +486,29 @@
           <t>test</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>k</t>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>hi</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve form submission feedback to users with status messages
Adds a status display div and associated CSS to provide user feedback on form submission success or failure. Updates JavaScript to dynamically show and hide these messages, replacing previous alerts, with a timeout for automatic dismissal.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: aa1355a6-4859-4c24-8204-39ae879ef4a6
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/71061587-a7b1-4597-9e8f-9df05ef5f8e3/aa1355a6-4859-4c24-8204-39ae879ef4a6/9cIJIDv
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,14 +501,29 @@
           <t>test</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="B5" t="n">
+        <v>30</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>j</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve user feedback messages and update viewport settings
Update index.html to refine user feedback messages for submission status (success/error) and adjust the viewport meta tag.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: aa1355a6-4859-4c24-8204-39ae879ef4a6
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/71061587-a7b1-4597-9e8f-9df05ef5f8e3/aa1355a6-4859-4c24-8204-39ae879ef4a6/9cIJIDv
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,14 +516,44 @@
           <t>h</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B6" t="n">
+        <v>20</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>j</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>gb</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>22</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>